<commit_message>
Glider 312 deployment 00003. Added deployed ingest sheet and cal sheet. Also made minor edit to 311 00002 cal sheet.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL311/Omaha_Cal_Info_CE05MOAS-GL311_00002.xlsx
+++ b/CE05MOAS-GL311/Omaha_Cal_Info_CE05MOAS-GL311_00002.xlsx
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
         <v>42391</v>
       </c>
       <c r="E2" s="25">
-        <v>0.94791666666666663</v>
+        <v>0.86458333333333337</v>
       </c>
       <c r="F2" s="23"/>
       <c r="G2" s="16" t="s">

</xml_diff>